<commit_message>
Notes du TP1 pour TPA1 et TPA3
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S3/R3-03-Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-Info-R-03-Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F75BEA6-931C-0641-BAD6-F6320DEC4CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B76F212-5476-4D62-ABE7-C5379CF5AB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="34960" windowHeight="20300" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +83,31 @@
   <si>
     <t>La deuxième question elaastic sur l'exigence 3.4 est trop difficile en question ouverte pour des novices : une question fermée avec commes choix ("Exigence projet", "Contrainte réglementaire", "Exigence qualité", "Exigence transverse") serait mieux. Insister sur le caractère non finissable de l'exigence transverce. ce qui fait qu'elle ne peut pas aller dans le backlog (elle ira dans la définition de fini).
 La 3ème question sur les exigences projet a bien fonctionné : la réponse chat GPT 4 est tellement bonne que je l'ai fournie comme une réponse élève.</t>
+  </si>
+  <si>
+    <t>MPAL</t>
+  </si>
+  <si>
+    <t>Lecture active du CDC, mise en commun en binome. 2 questions Elaastic.</t>
+  </si>
+  <si>
+    <t>Lecture active du CDC, mise en commun en binome. 3 questions Elaastic.</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Ce qui est ressorti des discussion : pas d'exigences liées à l'ergonomie ou l'architecture hierarchique du site. Clarification de l'obtention du niveau de privilège. Mise en commun avec la classe et les très bonnes questions soulevées ont amené à devancer un peu les questions Elaastic...
+Elaastic 1 : Peu de réponses liées au caractère évolutif et imprécis du CDC, qu'il faudrait transformer en US. Plutôt tendance à dire qu'il faut modifier le CDC.
+Elaastic 2 : Peu efficace. Surtout des réponses liées au fait qu'il ne s'agissait pas d'une fonctionnalité mais d'une notion de compatibilité. Personne n'a soulevé la notion de fonctionnalité/exigence transversale et non finissable.</t>
+  </si>
+  <si>
+    <t>Discussions : beaucoup de questionnements. 
+Certains ne voient pas ce qui cloche : "c'est normal de se poser des questions, on y répondra au fur et à mesure avec le client car méthode Agile")
+Pas de mise en commun des questionnements avant Elaastic.
+Elaastic 1 : tout le monde est d'accord pour dire que le CDC est imprécis. Les meilleurs notes disent ce qu'il manque. Peu disent que c'est normal et que la méthode Agile servira à clarifier. 
+Elaastic 2 : bon repérage du caractère non fonctionnel, mais peu disent la notion de non finissable. Certain confondent exigence qualité, technique, accessibilité...
+Elaastic 3 : remarque générale sur la durée de développement, mais pas sur la couverture fonctionnelle de 100%.</t>
   </si>
 </sst>
 </file>
@@ -138,7 +161,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -152,10 +178,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -181,17 +207,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{545EC486-0A2C-2E4F-BF0F-46D1FEA28E93}" name="Tableau1" displayName="Tableau1" ref="A1:H31" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:H31" xr:uid="{545EC486-0A2C-2E4F-BF0F-46D1FEA28E93}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{545EC486-0A2C-2E4F-BF0F-46D1FEA28E93}" name="Tableau1" displayName="Tableau1" ref="A1:I31" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:I31" xr:uid="{545EC486-0A2C-2E4F-BF0F-46D1FEA28E93}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F071AF06-C197-6349-9335-A3F4CE2613C5}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{781EEA16-EEF6-234E-8C83-429967F6CD67}" name="Enseignant" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{CE2A7765-53E4-144E-A997-283079C0546E}" name="Séance" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{5D953C1E-59E3-8142-B0DB-D1F53D00314F}" name="Groupe A1" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{4CD3C238-1456-EA42-BC8E-5C8980B8F66F}" name="Groupe A2-4" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{C755FE14-1AF3-0949-991C-3E8940F6D06E}" name="Groupe A3" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{C1154B8C-A2A9-E945-829D-2C3F5D7DDDE3}" name="Description" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{B4CB543C-BD2C-FB42-8582-C90EB201607D}" name="Améliortions pour l'année prochaine" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{C755FE14-1AF3-0949-991C-3E8940F6D06E}" name="Groupe A3" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C1154B8C-A2A9-E945-829D-2C3F5D7DDDE3}" name="Description" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{B4CB543C-BD2C-FB42-8582-C90EB201607D}" name="Améliortions pour l'année prochaine" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{92EC0337-3204-409E-9777-A3C035E8C35F}" name="Commentaires" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -494,13 +521,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CB8932-8F77-664F-AF33-70DF36E0AE91}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
@@ -509,9 +536,10 @@
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="41.33203125" customWidth="1"/>
     <col min="8" max="8" width="46" customWidth="1"/>
+    <col min="9" max="9" width="79.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,8 +564,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
@@ -562,8 +593,9 @@
       <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="187" x14ac:dyDescent="0.2">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -582,28 +614,55 @@
       <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>45181</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="I4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="155" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>45181</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -612,8 +671,9 @@
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -622,8 +682,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -632,8 +693,9 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -642,8 +704,9 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -652,8 +715,9 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -662,8 +726,9 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -672,8 +737,9 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -682,8 +748,9 @@
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -692,8 +759,9 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -702,8 +770,9 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -712,8 +781,9 @@
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -722,8 +792,9 @@
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -732,8 +803,9 @@
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -742,8 +814,9 @@
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -752,8 +825,9 @@
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -762,8 +836,9 @@
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -772,8 +847,9 @@
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -782,8 +858,9 @@
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -792,8 +869,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -802,8 +880,9 @@
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -812,8 +891,9 @@
       <c r="F26" s="3"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -822,8 +902,9 @@
       <c r="F27" s="3"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -832,8 +913,9 @@
       <c r="F28" s="3"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -842,8 +924,9 @@
       <c r="F29" s="3"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -852,8 +935,9 @@
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -862,6 +946,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
+      <c r="I31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MAJ suite au séances du 18/09
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-Info-R-03-Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S3/R3-03-Analyse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B76F212-5476-4D62-ABE7-C5379CF5AB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BFA121-BA08-9045-805C-3F62D407B746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24520" windowHeight="12760" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -109,13 +109,55 @@
 Elaastic 2 : bon repérage du caractère non fonctionnel, mais peu disent la notion de non finissable. Certain confondent exigence qualité, technique, accessibilité...
 Elaastic 3 : remarque générale sur la durée de développement, mais pas sur la couverture fonctionnelle de 100%.</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Quizz, rapppel pndant 1h, essentiel, vu les résultats. Puis fin présentation partie US sans les tests d'acceptations puis présentation des diapo sur ce qu'est lanayse métier.</t>
+  </si>
+  <si>
+    <r>
+      <t>Inscription assignment Github classroom. J'ai fait préfixé le nom d'équipe par "G</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" ou N est numéro du groupe.
+Prise en main de Github Issues et Github projects (sans lien avec le code source) en mode "kata" : je fais les manip, ils suivent en pas à pas. Attention parfois de bien clairifier qu'un seul membre doit faire la manip.
+Activité de rédaction des US sur la dernière demi-heure. Les 8 dernières minutes, certains ont pu commencer à mettre des commentaires sur les US des autres en utilisant les commentaires sur l'interface de consultation d'une issue.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -523,11 +565,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CB8932-8F77-664F-AF33-70DF36E0AE91}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
@@ -536,10 +578,10 @@
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="41.33203125" customWidth="1"/>
     <col min="8" max="8" width="46" customWidth="1"/>
-    <col min="9" max="9" width="79.75" customWidth="1"/>
+    <col min="9" max="9" width="79.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
@@ -595,7 +637,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -616,7 +658,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45181</v>
       </c>
@@ -639,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="155" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45181</v>
       </c>
@@ -662,29 +704,51 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
+    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>45187</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="238" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -695,7 +759,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -706,7 +770,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -717,7 +781,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -728,7 +792,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -739,7 +803,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -750,7 +814,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -761,7 +825,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -772,7 +836,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -783,7 +847,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -794,7 +858,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -805,7 +869,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -816,7 +880,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -827,7 +891,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -838,7 +902,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -849,7 +913,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -860,7 +924,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -871,7 +935,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -882,7 +946,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -893,7 +957,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -904,7 +968,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -915,7 +979,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -926,7 +990,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -937,7 +1001,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
TPA1 CR de séance
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S3/R3-03-Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-Info-R-03-Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BFA121-BA08-9045-805C-3F62D407B746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D585277E-F32D-4D62-BC46-54B20729636C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24520" windowHeight="12760" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -142,6 +142,12 @@
 Prise en main de Github Issues et Github projects (sans lien avec le code source) en mode "kata" : je fais les manip, ils suivent en pas à pas. Attention parfois de bien clairifier qu'un seul membre doit faire la manip.
 Activité de rédaction des US sur la dernière demi-heure. Les 8 dernières minutes, certains ont pu commencer à mettre des commentaires sur les US des autres en utilisant les commentaires sur l'interface de consultation d'une issue.</t>
     </r>
+  </si>
+  <si>
+    <t>45min de prise en main de Issues, Classroom et Projects, 30min de rédaction des US.</t>
+  </si>
+  <si>
+    <t>Difficulté à différencier le point d'entrée Classroom vs le dépôt Github.</t>
   </si>
 </sst>
 </file>
@@ -565,11 +571,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CB8932-8F77-664F-AF33-70DF36E0AE91}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
@@ -581,7 +587,7 @@
     <col min="9" max="9" width="79.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
@@ -637,7 +643,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -658,7 +664,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45181</v>
       </c>
@@ -681,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="155" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45181</v>
       </c>
@@ -704,7 +710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45187</v>
       </c>
@@ -729,7 +735,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -748,18 +754,28 @@
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -770,7 +786,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -781,7 +797,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -792,7 +808,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -803,7 +819,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -814,7 +830,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -825,7 +841,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -836,7 +852,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -847,7 +863,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -858,7 +874,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -869,7 +885,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -880,7 +896,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -891,7 +907,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -902,7 +918,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -913,7 +929,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -924,7 +940,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -935,7 +951,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -946,7 +962,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -957,7 +973,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -968,7 +984,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -979,7 +995,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -990,7 +1006,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1001,7 +1017,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
TPA3 et TPA1 CR du 28/09/2023
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S3/R3-03-Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-Info-R-03-Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D9D481-BA93-B741-94B0-C8B9E7238C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C676BF-C74A-44E4-AF43-2D5D21A7ECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23420" windowHeight="13600" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -165,6 +165,12 @@
     <t>Écriture des US en binomes terminée (30mn). J'ai demandé aux binomes qui avaient des doutes sur leurs US de se signaler pour aller voir ces US. 2 tiers des biomes avaient des doutes. C'était donc bien de déminer... Pendant que je circulais les questions Elaastic étaient lancées pour que tout le monde ait de quoi faire.
 Activités sur Elaastic, exemples tests d'acceptation (45mn). La dernière question a été traitée directement en insistant sur le fait qu'il est pertinent de sortir les règles métier des tests d'acceptation.
 Lien de partage enseignant de l'activité de tests : https://elaastic.irit.fr:443/elaastic-questions/subject/shared?globalId=c447e876-f562-4d2f-91ba-45c048dbfac6</t>
+  </si>
+  <si>
+    <t>Fin d'écriture des US puis échange des US pour correction par l'autre membre. J'ai consulté au hasard des US de chaque groupe pour un faire un retour général sur les critères INVEST et les 3C. 45 minutes. Ensuite, début de travail sur les tests d'accepation. L'activité elaastic n'a pu être lancée que dans les 10 dernières minutes par manque de planification de ma part (j'avais oublié de créer l'activité Moodle et de créer une diffusion dans elaastic). Seul la phase 1 de la question a été faite.</t>
+  </si>
+  <si>
+    <t>45 minutes d'échanges et de travail sur la rédaction des US, retour sur les critères INVEST. Activité elaastic : question 1 faite en entier : retour intéressant : dans les meilleures réponses on trouve : Tout est cas nominal sauf "Impossible to delete non empty course". Mais aussi : "Delete Confirmed" est le cas nominal mais "Delete Cancelled" et "Impossible to delete non empty course". Nous avons discuté donc de savoir si "Delete Cancelled" était du nominal ou non.</t>
   </si>
 </sst>
 </file>
@@ -588,11 +594,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CB8932-8F77-664F-AF33-70DF36E0AE91}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
@@ -604,7 +610,7 @@
     <col min="9" max="9" width="79.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
@@ -660,7 +666,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -681,7 +687,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45181</v>
       </c>
@@ -704,7 +710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="155" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45181</v>
       </c>
@@ -727,7 +733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45187</v>
       </c>
@@ -752,7 +758,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -771,7 +777,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45190</v>
       </c>
@@ -794,7 +800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45190</v>
       </c>
@@ -817,7 +823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45194</v>
       </c>
@@ -844,7 +850,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="248" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45194</v>
       </c>
@@ -863,29 +869,49 @@
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+    <row r="12" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>45197</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+    <row r="13" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>45197</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -896,7 +922,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -907,7 +933,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -918,7 +944,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -929,7 +955,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -940,7 +966,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -951,7 +977,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -962,7 +988,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -973,7 +999,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -984,7 +1010,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -995,7 +1021,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1006,7 +1032,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1017,7 +1043,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1028,7 +1054,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1039,7 +1065,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1050,7 +1076,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1061,7 +1087,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1072,7 +1098,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
TPA1 et TPA3 US
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S3/R3-03-Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-Info-R-03-Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F867F6-3A8C-0A40-B83D-8814D077073C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAE702A-9742-4769-A034-A72130022352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13920" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -193,6 +193,26 @@
   </si>
   <si>
     <t>Travail sur tests d'acceptation à rédiger. Ils ont fini par rédiger plein de tests sur leurs US : le passage dans les rangs pour échanger a été important. J'ai aussi insister au départ sur le fait qu'ils devaient s'inspirer des exemples résolus.</t>
+  </si>
+  <si>
+    <t>Reformulation de la question elaastic 3 ?</t>
+  </si>
+  <si>
+    <t>Elaastic : question 2 et 3 : difficulté du groupe à comprendre la signification de la question 3 "comment aurait pu être traitée" ne leur semble pas très clair.
+Suite des rédactions des Tests d'Acceptation : remarques fréquentes sur des éléments du When qui pourraient en fait être placés dans le Given : "Given : Un membre non connecté sur la page de connexion
+When : il clique sur le bouton de connexion après avoir correctement rempli ses informations
+Then : il est connecté"
+Le "après avoir correctement rempli ses informations" devrait être placé dans le Given ?</t>
+  </si>
+  <si>
+    <t>Elaastic : fin de l'activité + Rédaction de Tests d'acceptation. Pourrait-on envisager d'avoir des Business Rules et Lexique externe à toutes US pour préciser le type de visiteur ? Exemple :
+"Business Rule : types d'utilisateur
+Il y a 4 types d'utilisateurs du site ALOSA :
+- visiteur : un internaute non authentifié
+- membre : internaute authentifié bénéficiant de permissions standard
+- membre expert : internaute authentifié bénéficiant de permissions expert
+- administrateur : internaute authentifié bénéficiant de permissions administrateur
+"</t>
   </si>
 </sst>
 </file>
@@ -616,11 +636,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CB8932-8F77-664F-AF33-70DF36E0AE91}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
@@ -632,7 +652,7 @@
     <col min="9" max="9" width="79.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -661,7 +681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
@@ -688,7 +708,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -709,7 +729,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45181</v>
       </c>
@@ -732,7 +752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="155" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45181</v>
       </c>
@@ -755,7 +775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45187</v>
       </c>
@@ -780,7 +800,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -799,7 +819,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45190</v>
       </c>
@@ -822,7 +842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45190</v>
       </c>
@@ -845,7 +865,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45194</v>
       </c>
@@ -872,7 +892,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="248" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45194</v>
       </c>
@@ -891,7 +911,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45197</v>
       </c>
@@ -912,7 +932,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45197</v>
       </c>
@@ -933,7 +953,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45201</v>
       </c>
@@ -960,7 +980,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -981,7 +1001,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
@@ -1000,29 +1020,51 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+    <row r="17" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>45204</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+    <row r="18" spans="1:9" ht="217" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>45204</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1033,7 +1075,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1044,7 +1086,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1055,7 +1097,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1066,7 +1108,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1077,7 +1119,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1088,7 +1130,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1099,7 +1141,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1110,7 +1152,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1121,7 +1163,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1132,7 +1174,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1143,7 +1185,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1154,7 +1196,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
Préparation du Journal de Bord pour jeudi 12/10
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S3/R3-03-Analyse/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BF6174-8850-494A-A5C7-0E5EB20D9658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27680" windowHeight="15680" xr2:uid="{B5A40BE9-EAD0-F247-87B3-754BF66AB48F}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="27675" windowHeight="15675"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -227,8 +221,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,35 +279,35 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -329,18 +323,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{545EC486-0A2C-2E4F-BF0F-46D1FEA28E93}" name="Tableau1" displayName="Tableau1" ref="A1:I31" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:I31" xr:uid="{545EC486-0A2C-2E4F-BF0F-46D1FEA28E93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I31" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:I31"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{F071AF06-C197-6349-9335-A3F4CE2613C5}" name="Date" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{781EEA16-EEF6-234E-8C83-429967F6CD67}" name="Enseignant" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{CE2A7765-53E4-144E-A997-283079C0546E}" name="Séance" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{5D953C1E-59E3-8142-B0DB-D1F53D00314F}" name="Groupe A1" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4CD3C238-1456-EA42-BC8E-5C8980B8F66F}" name="Groupe A2-4" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{C755FE14-1AF3-0949-991C-3E8940F6D06E}" name="Groupe A3" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{C1154B8C-A2A9-E945-829D-2C3F5D7DDDE3}" name="Description" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{B4CB543C-BD2C-FB42-8582-C90EB201607D}" name="Améliortions pour l'année prochaine" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{92EC0337-3204-409E-9777-A3C035E8C35F}" name="Commentaires" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="8"/>
+    <tableColumn id="2" name="Enseignant" dataDxfId="7"/>
+    <tableColumn id="3" name="Séance" dataDxfId="6"/>
+    <tableColumn id="4" name="Groupe A1" dataDxfId="5"/>
+    <tableColumn id="5" name="Groupe A2-4" dataDxfId="4"/>
+    <tableColumn id="6" name="Groupe A3" dataDxfId="3"/>
+    <tableColumn id="7" name="Description" dataDxfId="2"/>
+    <tableColumn id="8" name="Améliortions pour l'année prochaine" dataDxfId="1"/>
+    <tableColumn id="9" name="Commentaires" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -389,7 +383,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -441,7 +435,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -635,33 +629,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CB8932-8F77-664F-AF33-70DF36E0AE91}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="1" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="41.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
+    <col min="7" max="7" width="41.375" customWidth="1"/>
     <col min="8" max="8" width="46" customWidth="1"/>
-    <col min="9" max="9" width="79.6640625" customWidth="1"/>
+    <col min="9" max="9" width="79.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="47.25">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
@@ -717,7 +711,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="173.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -738,7 +732,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="141.75">
       <c r="A4" s="2">
         <v>45181</v>
       </c>
@@ -761,7 +755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="157.5">
       <c r="A5" s="2">
         <v>45181</v>
       </c>
@@ -784,7 +778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="63">
       <c r="A6" s="2">
         <v>45187</v>
       </c>
@@ -809,7 +803,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="204.75">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -828,7 +822,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="31.5">
       <c r="A8" s="2">
         <v>45190</v>
       </c>
@@ -851,7 +845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="31.5">
       <c r="A9" s="2">
         <v>45190</v>
       </c>
@@ -874,7 +868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="63">
       <c r="A10" s="2">
         <v>45194</v>
       </c>
@@ -901,7 +895,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="252">
       <c r="A11" s="2">
         <v>45194</v>
       </c>
@@ -920,7 +914,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="173.25">
       <c r="A12" s="2">
         <v>45197</v>
       </c>
@@ -941,7 +935,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="173.25">
       <c r="A13" s="2">
         <v>45197</v>
       </c>
@@ -962,7 +956,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="220.5">
       <c r="A14" s="2">
         <v>45201</v>
       </c>
@@ -989,7 +983,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -1010,7 +1004,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="78.75">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
@@ -1029,7 +1023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="255" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="220.5">
       <c r="A17" s="2">
         <v>45204</v>
       </c>
@@ -1052,7 +1046,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="220.5">
       <c r="A18" s="2">
         <v>45204</v>
       </c>
@@ -1073,7 +1067,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="63">
       <c r="A19" s="2">
         <v>45208</v>
       </c>
@@ -1098,29 +1092,45 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2">
+        <v>45211</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+    <row r="21" spans="1:9">
+      <c r="A21" s="2">
+        <v>45211</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1131,7 +1141,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1142,7 +1152,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1153,7 +1163,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1164,7 +1174,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1175,7 +1185,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1186,7 +1196,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1197,7 +1207,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1208,7 +1218,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1219,7 +1229,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
Activité 3 DdF TPA3 du 16/10
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S3/R3-03-Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-Info-R-03-Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B890149C-C578-A044-AB12-F8E9F0E1800C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AC47C0-39BC-476A-804A-97C97447D9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="3440" windowWidth="29960" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -231,6 +231,18 @@
   </si>
   <si>
     <t>OK. Un étudiant a produit une réponse disant que l'écriture d'une Business Rule permettait de s'affranchir d'écrire les TA associés.</t>
+  </si>
+  <si>
+    <t>Bilan et synthèse autour de l'utilisation des Business Rules vs Tests d'Acceptation.
+Activité 3 : Définition de Fini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projet Web de la SAE pas encore lancé. Travaillé sur le projet Java de la SAE.
+Question : "Les tests unitaires passent" et "Les tests d'acceptation passent" vs "Au moins 80% de couverture fonctionnelle"?
+Je ne vois pas l'intérêt de dire que tous 100% des tests unitaires écrits passent : si certains ne passent pas, on les supprime et on arrive à nouveau à 100%...
+Pour 100% des tests d'acceptation : ne pas les respecter reviendrait à ne pas terminer l'implémentation de l'US non ? ce qui me parait étrange...
+Par ailleurs, pourrait-tu m'aider à clarifier ce qui signifie le niveau de couverture par les tests ? est-ce équivalent à la couverture fonctionnelle ?
+</t>
   </si>
 </sst>
 </file>
@@ -654,11 +666,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="H21" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
@@ -670,7 +682,7 @@
     <col min="9" max="9" width="79.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
@@ -726,7 +738,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -747,7 +759,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45181</v>
       </c>
@@ -770,7 +782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="155" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45181</v>
       </c>
@@ -793,7 +805,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45187</v>
       </c>
@@ -818,7 +830,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -837,7 +849,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45190</v>
       </c>
@@ -860,7 +872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45190</v>
       </c>
@@ -883,7 +895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45194</v>
       </c>
@@ -910,7 +922,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="248" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45194</v>
       </c>
@@ -929,7 +941,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45197</v>
       </c>
@@ -950,7 +962,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45197</v>
       </c>
@@ -971,7 +983,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45201</v>
       </c>
@@ -998,7 +1010,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -1019,7 +1031,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
@@ -1038,7 +1050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="255" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45204</v>
       </c>
@@ -1061,7 +1073,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="217" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45204</v>
       </c>
@@ -1082,7 +1094,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45208</v>
       </c>
@@ -1107,7 +1119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="93" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45211</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45211</v>
       </c>
@@ -1155,18 +1167,30 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+    <row r="22" spans="1:9" ht="155" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>45215</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="H22" s="4"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1177,7 +1201,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1188,7 +1212,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1199,7 +1223,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1210,7 +1234,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1221,7 +1245,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1232,7 +1256,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1243,7 +1267,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1254,7 +1278,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>